<commit_message>
More complete and sensible data in initial data files
</commit_message>
<xml_diff>
--- a/backend/src/main/resources/initialDataFiles/doses.xlsx
+++ b/backend/src/main/resources/initialDataFiles/doses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Java\SpringBootProjects\medtracker_v2_rest_api\backend\src\main\resources\initialDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834FC584-D404-4B11-BC36-20218B282A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29B3B38-5C74-465B-8EB4-A1243781A99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="876" windowWidth="46296" windowHeight="25212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18048" yWindow="5484" windowWidth="23676" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="7">
   <si>
     <t>Taken</t>
   </si>
@@ -376,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80:E196"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78:XFD78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1712,7 +1712,7 @@
         <v>1</v>
       </c>
       <c r="E78" s="4">
-        <v>0.37847222222222221</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -1732,9 +1732,2764 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" s="2">
+        <v>45629</v>
+      </c>
+      <c r="B80" s="1">
+        <v>4</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D80" t="b">
+        <v>1</v>
+      </c>
+      <c r="E80" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" s="2">
+        <v>45629</v>
+      </c>
+      <c r="B81" s="1">
+        <v>4</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D81" t="b">
+        <v>1</v>
+      </c>
+      <c r="E81" s="4">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" s="2">
+        <v>45630</v>
+      </c>
+      <c r="B82" s="1">
+        <v>4</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" t="b">
+        <v>1</v>
+      </c>
+      <c r="E82" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" s="2">
+        <v>45630</v>
+      </c>
+      <c r="B83" s="1">
+        <v>4</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D83" t="b">
+        <v>1</v>
+      </c>
+      <c r="E83" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" s="2">
+        <v>45631</v>
+      </c>
+      <c r="B84" s="1">
+        <v>4</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D84" t="b">
+        <v>1</v>
+      </c>
+      <c r="E84" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" s="2">
+        <v>45631</v>
+      </c>
+      <c r="B85" s="1">
+        <v>4</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D85" t="b">
+        <v>1</v>
+      </c>
+      <c r="E85" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" s="2">
+        <v>45632</v>
+      </c>
+      <c r="B86" s="1">
+        <v>4</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D86" t="b">
+        <v>1</v>
+      </c>
+      <c r="E86" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" s="2">
+        <v>45632</v>
+      </c>
+      <c r="B87" s="1">
+        <v>4</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D87" t="b">
+        <v>1</v>
+      </c>
+      <c r="E87" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" s="2">
+        <v>45633</v>
+      </c>
+      <c r="B88" s="1">
+        <v>4</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D88" t="b">
+        <v>1</v>
+      </c>
+      <c r="E88" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" s="2">
+        <v>45633</v>
+      </c>
+      <c r="B89" s="1">
+        <v>4</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D89" t="b">
+        <v>1</v>
+      </c>
+      <c r="E89" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" s="2">
+        <v>45634</v>
+      </c>
+      <c r="B90" s="1">
+        <v>4</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D90" t="b">
+        <v>1</v>
+      </c>
+      <c r="E90" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" s="2">
+        <v>45634</v>
+      </c>
+      <c r="B91" s="1">
+        <v>4</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D91" t="b">
+        <v>1</v>
+      </c>
+      <c r="E91" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" s="2">
+        <v>45635</v>
+      </c>
+      <c r="B92" s="1">
+        <v>4</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D92" t="b">
+        <v>1</v>
+      </c>
+      <c r="E92" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" s="2">
+        <v>45635</v>
+      </c>
+      <c r="B93" s="1">
+        <v>4</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D93" t="b">
+        <v>1</v>
+      </c>
+      <c r="E93" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" s="2">
+        <v>45636</v>
+      </c>
+      <c r="B94" s="1">
+        <v>4</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D94" t="b">
+        <v>1</v>
+      </c>
+      <c r="E94" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95" s="2">
+        <v>45636</v>
+      </c>
+      <c r="B95" s="1">
+        <v>4</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D95" t="b">
+        <v>1</v>
+      </c>
+      <c r="E95" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96" s="2">
+        <v>45637</v>
+      </c>
+      <c r="B96" s="1">
+        <v>4</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D96" t="b">
+        <v>1</v>
+      </c>
+      <c r="E96" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97" s="2">
+        <v>45637</v>
+      </c>
+      <c r="B97" s="1">
+        <v>4</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D97" t="b">
+        <v>1</v>
+      </c>
+      <c r="E97" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98" s="2">
+        <v>45638</v>
+      </c>
+      <c r="B98" s="1">
+        <v>4</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D98" t="b">
+        <v>1</v>
+      </c>
+      <c r="E98" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99" s="2">
+        <v>45638</v>
+      </c>
+      <c r="B99" s="1">
+        <v>4</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D99" t="b">
+        <v>1</v>
+      </c>
+      <c r="E99" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A100" s="2">
+        <v>45639</v>
+      </c>
+      <c r="B100" s="1">
+        <v>4</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D100" t="b">
+        <v>1</v>
+      </c>
+      <c r="E100" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A101" s="2">
+        <v>45639</v>
+      </c>
+      <c r="B101" s="1">
+        <v>4</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D101" t="b">
+        <v>1</v>
+      </c>
+      <c r="E101" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A102" s="2">
+        <v>45640</v>
+      </c>
+      <c r="B102" s="1">
+        <v>4</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D102" t="b">
+        <v>1</v>
+      </c>
+      <c r="E102" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A103" s="2">
+        <v>45640</v>
+      </c>
+      <c r="B103" s="1">
+        <v>4</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D103" t="b">
+        <v>1</v>
+      </c>
+      <c r="E103" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104" s="2">
+        <v>45641</v>
+      </c>
+      <c r="B104" s="1">
+        <v>4</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D104" t="b">
+        <v>1</v>
+      </c>
+      <c r="E104" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105" s="2">
+        <v>45641</v>
+      </c>
+      <c r="B105" s="1">
+        <v>4</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D105" t="b">
+        <v>1</v>
+      </c>
+      <c r="E105" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A106" s="2">
+        <v>45642</v>
+      </c>
+      <c r="B106" s="1">
+        <v>4</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D106" t="b">
+        <v>1</v>
+      </c>
+      <c r="E106" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A107" s="2">
+        <v>45642</v>
+      </c>
+      <c r="B107" s="1">
+        <v>4</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D107" t="b">
+        <v>1</v>
+      </c>
+      <c r="E107" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A108" s="2">
+        <v>45643</v>
+      </c>
+      <c r="B108" s="1">
+        <v>4</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D108" t="b">
+        <v>1</v>
+      </c>
+      <c r="E108" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A109" s="2">
+        <v>45643</v>
+      </c>
+      <c r="B109" s="1">
+        <v>4</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D109" t="b">
+        <v>1</v>
+      </c>
+      <c r="E109" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110" s="2">
+        <v>45644</v>
+      </c>
+      <c r="B110" s="1">
+        <v>4</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D110" t="b">
+        <v>1</v>
+      </c>
+      <c r="E110" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A111" s="2">
+        <v>45644</v>
+      </c>
+      <c r="B111" s="1">
+        <v>4</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D111" t="b">
+        <v>1</v>
+      </c>
+      <c r="E111" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A112" s="2">
+        <v>45645</v>
+      </c>
+      <c r="B112" s="1">
+        <v>4</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D112" t="b">
+        <v>1</v>
+      </c>
+      <c r="E112" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A113" s="2">
+        <v>45645</v>
+      </c>
+      <c r="B113" s="1">
+        <v>4</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D113" t="b">
+        <v>1</v>
+      </c>
+      <c r="E113" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A114" s="2">
+        <v>45646</v>
+      </c>
+      <c r="B114" s="1">
+        <v>4</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D114" t="b">
+        <v>1</v>
+      </c>
+      <c r="E114" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A115" s="2">
+        <v>45646</v>
+      </c>
+      <c r="B115" s="1">
+        <v>4</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D115" t="b">
+        <v>1</v>
+      </c>
+      <c r="E115" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A116" s="2">
+        <v>45647</v>
+      </c>
+      <c r="B116" s="1">
+        <v>4</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D116" t="b">
+        <v>1</v>
+      </c>
+      <c r="E116" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A117" s="2">
+        <v>45647</v>
+      </c>
+      <c r="B117" s="1">
+        <v>4</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D117" t="b">
+        <v>1</v>
+      </c>
+      <c r="E117" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A118" s="2">
+        <v>45648</v>
+      </c>
+      <c r="B118" s="1">
+        <v>4</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D118" t="b">
+        <v>1</v>
+      </c>
+      <c r="E118" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A119" s="2">
+        <v>45648</v>
+      </c>
+      <c r="B119" s="1">
+        <v>4</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D119" t="b">
+        <v>1</v>
+      </c>
+      <c r="E119" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A120" s="2">
+        <v>45649</v>
+      </c>
+      <c r="B120" s="1">
+        <v>4</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D120" t="b">
+        <v>1</v>
+      </c>
+      <c r="E120" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A121" s="2">
+        <v>45649</v>
+      </c>
+      <c r="B121" s="1">
+        <v>4</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D121" t="b">
+        <v>1</v>
+      </c>
+      <c r="E121" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A122" s="2">
+        <v>45650</v>
+      </c>
+      <c r="B122" s="1">
+        <v>4</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D122" t="b">
+        <v>1</v>
+      </c>
+      <c r="E122" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A123" s="2">
+        <v>45650</v>
+      </c>
+      <c r="B123" s="1">
+        <v>4</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D123" t="b">
+        <v>1</v>
+      </c>
+      <c r="E123" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A124" s="2">
+        <v>45651</v>
+      </c>
+      <c r="B124" s="1">
+        <v>4</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D124" t="b">
+        <v>1</v>
+      </c>
+      <c r="E124" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A125" s="2">
+        <v>45651</v>
+      </c>
+      <c r="B125" s="1">
+        <v>4</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D125" t="b">
+        <v>1</v>
+      </c>
+      <c r="E125" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A126" s="2">
+        <v>45652</v>
+      </c>
+      <c r="B126" s="1">
+        <v>4</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D126" t="b">
+        <v>1</v>
+      </c>
+      <c r="E126" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A127" s="2">
+        <v>45652</v>
+      </c>
+      <c r="B127" s="1">
+        <v>4</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D127" t="b">
+        <v>1</v>
+      </c>
+      <c r="E127" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A128" s="2">
+        <v>45653</v>
+      </c>
+      <c r="B128" s="1">
+        <v>4</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D128" t="b">
+        <v>1</v>
+      </c>
+      <c r="E128" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A129" s="2">
+        <v>45653</v>
+      </c>
+      <c r="B129" s="1">
+        <v>4</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D129" t="b">
+        <v>1</v>
+      </c>
+      <c r="E129" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A130" s="2">
+        <v>45654</v>
+      </c>
+      <c r="B130" s="1">
+        <v>4</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D130" t="b">
+        <v>1</v>
+      </c>
+      <c r="E130" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A131" s="2">
+        <v>45654</v>
+      </c>
+      <c r="B131" s="1">
+        <v>4</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D131" t="b">
+        <v>1</v>
+      </c>
+      <c r="E131" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A132" s="2">
+        <v>45655</v>
+      </c>
+      <c r="B132" s="1">
+        <v>4</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D132" t="b">
+        <v>1</v>
+      </c>
+      <c r="E132" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A133" s="2">
+        <v>45655</v>
+      </c>
+      <c r="B133" s="1">
+        <v>4</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D133" t="b">
+        <v>1</v>
+      </c>
+      <c r="E133" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A134" s="2">
+        <v>45656</v>
+      </c>
+      <c r="B134" s="1">
+        <v>4</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D134" t="b">
+        <v>1</v>
+      </c>
+      <c r="E134" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A135" s="2">
+        <v>45656</v>
+      </c>
+      <c r="B135" s="1">
+        <v>4</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D135" t="b">
+        <v>1</v>
+      </c>
+      <c r="E135" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A136" s="2">
+        <v>45657</v>
+      </c>
+      <c r="B136" s="1">
+        <v>4</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D136" t="b">
+        <v>1</v>
+      </c>
+      <c r="E136" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A137" s="2">
+        <v>45657</v>
+      </c>
+      <c r="B137" s="1">
+        <v>4</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D137" t="b">
+        <v>1</v>
+      </c>
+      <c r="E137" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A138" s="2">
+        <v>45658</v>
+      </c>
+      <c r="B138" s="1">
+        <v>4</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D138" t="b">
+        <v>1</v>
+      </c>
+      <c r="E138" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A139" s="2">
+        <v>45658</v>
+      </c>
+      <c r="B139" s="1">
+        <v>4</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D139" t="b">
+        <v>1</v>
+      </c>
+      <c r="E139" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A140" s="2">
+        <v>45659</v>
+      </c>
+      <c r="B140" s="1">
+        <v>4</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D140" t="b">
+        <v>1</v>
+      </c>
+      <c r="E140" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A141" s="2">
+        <v>45659</v>
+      </c>
+      <c r="B141" s="1">
+        <v>4</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D141" t="b">
+        <v>1</v>
+      </c>
+      <c r="E141" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A142" s="2">
+        <v>45660</v>
+      </c>
+      <c r="B142" s="1">
+        <v>4</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D142" t="b">
+        <v>1</v>
+      </c>
+      <c r="E142" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A143" s="2">
+        <v>45660</v>
+      </c>
+      <c r="B143" s="1">
+        <v>4</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D143" t="b">
+        <v>1</v>
+      </c>
+      <c r="E143" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A144" s="2">
+        <v>45661</v>
+      </c>
+      <c r="B144" s="1">
+        <v>4</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D144" t="b">
+        <v>1</v>
+      </c>
+      <c r="E144" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A145" s="2">
+        <v>45661</v>
+      </c>
+      <c r="B145" s="1">
+        <v>4</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D145" t="b">
+        <v>1</v>
+      </c>
+      <c r="E145" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A146" s="2">
+        <v>45662</v>
+      </c>
+      <c r="B146" s="1">
+        <v>4</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D146" t="b">
+        <v>1</v>
+      </c>
+      <c r="E146" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A147" s="2">
+        <v>45662</v>
+      </c>
+      <c r="B147" s="1">
+        <v>4</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D147" t="b">
+        <v>1</v>
+      </c>
+      <c r="E147" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A148" s="2">
+        <v>45663</v>
+      </c>
+      <c r="B148" s="1">
+        <v>4</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D148" t="b">
+        <v>1</v>
+      </c>
+      <c r="E148" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A149" s="2">
+        <v>45663</v>
+      </c>
+      <c r="B149" s="1">
+        <v>4</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D149" t="b">
+        <v>1</v>
+      </c>
+      <c r="E149" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A150" s="2">
+        <v>45664</v>
+      </c>
+      <c r="B150" s="1">
+        <v>4</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D150" t="b">
+        <v>1</v>
+      </c>
+      <c r="E150" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A151" s="2">
+        <v>45664</v>
+      </c>
+      <c r="B151" s="1">
+        <v>4</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D151" t="b">
+        <v>1</v>
+      </c>
+      <c r="E151" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A152" s="2">
+        <v>45665</v>
+      </c>
+      <c r="B152" s="1">
+        <v>4</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D152" t="b">
+        <v>1</v>
+      </c>
+      <c r="E152" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A153" s="2">
+        <v>45665</v>
+      </c>
+      <c r="B153" s="1">
+        <v>4</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D153" t="b">
+        <v>1</v>
+      </c>
+      <c r="E153" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A154" s="2">
+        <v>45666</v>
+      </c>
+      <c r="B154" s="1">
+        <v>4</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D154" t="b">
+        <v>1</v>
+      </c>
+      <c r="E154" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A155" s="2">
+        <v>45666</v>
+      </c>
+      <c r="B155" s="1">
+        <v>4</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D155" t="b">
+        <v>1</v>
+      </c>
+      <c r="E155" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A156" s="2">
+        <v>45667</v>
+      </c>
+      <c r="B156" s="1">
+        <v>4</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D156" t="b">
+        <v>1</v>
+      </c>
+      <c r="E156" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A157" s="2">
+        <v>45667</v>
+      </c>
+      <c r="B157" s="1">
+        <v>4</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D157" t="b">
+        <v>1</v>
+      </c>
+      <c r="E157" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A158" s="2">
+        <v>45668</v>
+      </c>
+      <c r="B158" s="1">
+        <v>4</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D158" t="b">
+        <v>1</v>
+      </c>
+      <c r="E158" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A159" s="2">
+        <v>45668</v>
+      </c>
+      <c r="B159" s="1">
+        <v>4</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D159" t="b">
+        <v>1</v>
+      </c>
+      <c r="E159" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A160" s="2">
+        <v>45669</v>
+      </c>
+      <c r="B160" s="1">
+        <v>4</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D160" t="b">
+        <v>1</v>
+      </c>
+      <c r="E160" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A161" s="2">
+        <v>45669</v>
+      </c>
+      <c r="B161" s="1">
+        <v>4</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D161" t="b">
+        <v>1</v>
+      </c>
+      <c r="E161" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A162" s="2">
+        <v>45670</v>
+      </c>
+      <c r="B162" s="1">
+        <v>4</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D162" t="b">
+        <v>1</v>
+      </c>
+      <c r="E162" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A163" s="2">
+        <v>45670</v>
+      </c>
+      <c r="B163" s="1">
+        <v>4</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D163" t="b">
+        <v>1</v>
+      </c>
+      <c r="E163" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A164" s="2">
+        <v>45671</v>
+      </c>
+      <c r="B164" s="1">
+        <v>4</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D164" t="b">
+        <v>1</v>
+      </c>
+      <c r="E164" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A165" s="2">
+        <v>45671</v>
+      </c>
+      <c r="B165" s="1">
+        <v>4</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D165" t="b">
+        <v>1</v>
+      </c>
+      <c r="E165" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A166" s="2">
+        <v>45672</v>
+      </c>
+      <c r="B166" s="1">
+        <v>4</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D166" t="b">
+        <v>1</v>
+      </c>
+      <c r="E166" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A167" s="2">
+        <v>45672</v>
+      </c>
+      <c r="B167" s="1">
+        <v>4</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D167" t="b">
+        <v>1</v>
+      </c>
+      <c r="E167" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A168" s="2">
+        <v>45673</v>
+      </c>
+      <c r="B168" s="1">
+        <v>4</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D168" t="b">
+        <v>1</v>
+      </c>
+      <c r="E168" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A169" s="2">
+        <v>45673</v>
+      </c>
+      <c r="B169" s="1">
+        <v>4</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D169" t="b">
+        <v>1</v>
+      </c>
+      <c r="E169" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A170" s="2">
+        <v>45674</v>
+      </c>
+      <c r="B170" s="1">
+        <v>4</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D170" t="b">
+        <v>1</v>
+      </c>
+      <c r="E170" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A171" s="2">
+        <v>45674</v>
+      </c>
+      <c r="B171" s="1">
+        <v>4</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D171" t="b">
+        <v>1</v>
+      </c>
+      <c r="E171" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A172" s="2">
+        <v>45675</v>
+      </c>
+      <c r="B172" s="1">
+        <v>4</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D172" t="b">
+        <v>1</v>
+      </c>
+      <c r="E172" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A173" s="2">
+        <v>45675</v>
+      </c>
+      <c r="B173" s="1">
+        <v>4</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D173" t="b">
+        <v>1</v>
+      </c>
+      <c r="E173" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A174" s="2">
+        <v>45676</v>
+      </c>
+      <c r="B174" s="1">
+        <v>4</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D174" t="b">
+        <v>1</v>
+      </c>
+      <c r="E174" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A175" s="2">
+        <v>45676</v>
+      </c>
+      <c r="B175" s="1">
+        <v>4</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D175" t="b">
+        <v>1</v>
+      </c>
+      <c r="E175" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A176" s="2">
+        <v>45677</v>
+      </c>
+      <c r="B176" s="1">
+        <v>4</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D176" t="b">
+        <v>1</v>
+      </c>
+      <c r="E176" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A177" s="2">
+        <v>45677</v>
+      </c>
+      <c r="B177" s="1">
+        <v>4</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D177" t="b">
+        <v>1</v>
+      </c>
+      <c r="E177" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A178" s="2">
+        <v>45678</v>
+      </c>
+      <c r="B178" s="1">
+        <v>4</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D178" t="b">
+        <v>1</v>
+      </c>
+      <c r="E178" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A179" s="2">
+        <v>45678</v>
+      </c>
+      <c r="B179" s="1">
+        <v>4</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D179" t="b">
+        <v>1</v>
+      </c>
+      <c r="E179" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A180" s="2">
+        <v>45679</v>
+      </c>
+      <c r="B180" s="1">
+        <v>4</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D180" t="b">
+        <v>1</v>
+      </c>
+      <c r="E180" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A181" s="2">
+        <v>45679</v>
+      </c>
+      <c r="B181" s="1">
+        <v>4</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D181" t="b">
+        <v>1</v>
+      </c>
+      <c r="E181" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A182" s="2">
+        <v>45680</v>
+      </c>
+      <c r="B182" s="1">
+        <v>4</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D182" t="b">
+        <v>1</v>
+      </c>
+      <c r="E182" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A183" s="2">
+        <v>45680</v>
+      </c>
+      <c r="B183" s="1">
+        <v>4</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D183" t="b">
+        <v>1</v>
+      </c>
+      <c r="E183" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A184" s="2">
+        <v>45681</v>
+      </c>
+      <c r="B184" s="1">
+        <v>4</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D184" t="b">
+        <v>1</v>
+      </c>
+      <c r="E184" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A185" s="2">
+        <v>45681</v>
+      </c>
+      <c r="B185" s="1">
+        <v>4</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D185" t="b">
+        <v>1</v>
+      </c>
+      <c r="E185" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A186" s="2">
+        <v>45682</v>
+      </c>
+      <c r="B186" s="1">
+        <v>4</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D186" t="b">
+        <v>1</v>
+      </c>
+      <c r="E186" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A187" s="2">
+        <v>45682</v>
+      </c>
+      <c r="B187" s="1">
+        <v>4</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D187" t="b">
+        <v>1</v>
+      </c>
+      <c r="E187" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A188" s="2">
+        <v>45683</v>
+      </c>
+      <c r="B188" s="1">
+        <v>4</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D188" t="b">
+        <v>1</v>
+      </c>
+      <c r="E188" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A189" s="2">
+        <v>45683</v>
+      </c>
+      <c r="B189" s="1">
+        <v>4</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D189" t="b">
+        <v>1</v>
+      </c>
+      <c r="E189" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A190" s="2">
+        <v>45684</v>
+      </c>
+      <c r="B190" s="1">
+        <v>4</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D190" t="b">
+        <v>1</v>
+      </c>
+      <c r="E190" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A191" s="2">
+        <v>45684</v>
+      </c>
+      <c r="B191" s="1">
+        <v>4</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D191" t="b">
+        <v>1</v>
+      </c>
+      <c r="E191" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A192" s="2">
+        <v>45685</v>
+      </c>
+      <c r="B192" s="1">
+        <v>4</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D192" t="b">
+        <v>1</v>
+      </c>
+      <c r="E192" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A193" s="2">
+        <v>45685</v>
+      </c>
+      <c r="B193" s="1">
+        <v>4</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D193" t="b">
+        <v>1</v>
+      </c>
+      <c r="E193" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A194" s="2">
+        <v>45686</v>
+      </c>
+      <c r="B194" s="1">
+        <v>4</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D194" t="b">
+        <v>1</v>
+      </c>
+      <c r="E194" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A195" s="2">
+        <v>45686</v>
+      </c>
+      <c r="B195" s="1">
+        <v>4</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D195" t="b">
+        <v>1</v>
+      </c>
+      <c r="E195" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A196" s="2">
+        <v>45687</v>
+      </c>
+      <c r="B196" s="1">
+        <v>4</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D196" t="b">
+        <v>1</v>
+      </c>
+      <c r="E196" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A197" s="2">
+        <v>45687</v>
+      </c>
+      <c r="B197" s="1">
+        <v>4</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D197" t="b">
+        <v>1</v>
+      </c>
+      <c r="E197" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A198" s="2">
+        <v>45688</v>
+      </c>
+      <c r="B198" s="1">
+        <v>4</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D198" t="b">
+        <v>1</v>
+      </c>
+      <c r="E198" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A199" s="2">
+        <v>45688</v>
+      </c>
+      <c r="B199" s="1">
+        <v>4</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D199" t="b">
+        <v>1</v>
+      </c>
+      <c r="E199" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A200" s="2">
+        <v>45689</v>
+      </c>
+      <c r="B200" s="1">
+        <v>4</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D200" t="b">
+        <v>1</v>
+      </c>
+      <c r="E200" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A201" s="2">
+        <v>45689</v>
+      </c>
+      <c r="B201" s="1">
+        <v>4</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D201" t="b">
+        <v>1</v>
+      </c>
+      <c r="E201" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A202" s="2">
+        <v>45690</v>
+      </c>
+      <c r="B202" s="1">
+        <v>4</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D202" t="b">
+        <v>1</v>
+      </c>
+      <c r="E202" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A203" s="2">
+        <v>45690</v>
+      </c>
+      <c r="B203" s="1">
+        <v>4</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D203" t="b">
+        <v>1</v>
+      </c>
+      <c r="E203" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A204" s="2">
+        <v>45691</v>
+      </c>
+      <c r="B204" s="1">
+        <v>4</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D204" t="b">
+        <v>1</v>
+      </c>
+      <c r="E204" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A205" s="2">
+        <v>45691</v>
+      </c>
+      <c r="B205" s="1">
+        <v>4</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D205" t="b">
+        <v>1</v>
+      </c>
+      <c r="E205" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A206" s="2">
+        <v>45692</v>
+      </c>
+      <c r="B206" s="1">
+        <v>4</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D206" t="b">
+        <v>1</v>
+      </c>
+      <c r="E206" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A207" s="2">
+        <v>45692</v>
+      </c>
+      <c r="B207" s="1">
+        <v>4</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D207" t="b">
+        <v>1</v>
+      </c>
+      <c r="E207" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A208" s="2">
+        <v>45693</v>
+      </c>
+      <c r="B208" s="1">
+        <v>4</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D208" t="b">
+        <v>1</v>
+      </c>
+      <c r="E208" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A209" s="2">
+        <v>45693</v>
+      </c>
+      <c r="B209" s="1">
+        <v>4</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D209" t="b">
+        <v>1</v>
+      </c>
+      <c r="E209" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A210" s="2">
+        <v>45694</v>
+      </c>
+      <c r="B210" s="1">
+        <v>4</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D210" t="b">
+        <v>1</v>
+      </c>
+      <c r="E210" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A211" s="2">
+        <v>45694</v>
+      </c>
+      <c r="B211" s="1">
+        <v>4</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D211" t="b">
+        <v>1</v>
+      </c>
+      <c r="E211" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A212" s="2">
+        <v>45695</v>
+      </c>
+      <c r="B212" s="1">
+        <v>4</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D212" t="b">
+        <v>1</v>
+      </c>
+      <c r="E212" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A213" s="2">
+        <v>45695</v>
+      </c>
+      <c r="B213" s="1">
+        <v>4</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D213" t="b">
+        <v>1</v>
+      </c>
+      <c r="E213" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A214" s="2">
+        <v>45696</v>
+      </c>
+      <c r="B214" s="1">
+        <v>4</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D214" t="b">
+        <v>1</v>
+      </c>
+      <c r="E214" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A215" s="2">
+        <v>45696</v>
+      </c>
+      <c r="B215" s="1">
+        <v>4</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D215" t="b">
+        <v>1</v>
+      </c>
+      <c r="E215" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A216" s="2">
+        <v>45697</v>
+      </c>
+      <c r="B216" s="1">
+        <v>4</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D216" t="b">
+        <v>1</v>
+      </c>
+      <c r="E216" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A217" s="2">
+        <v>45697</v>
+      </c>
+      <c r="B217" s="1">
+        <v>4</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D217" t="b">
+        <v>1</v>
+      </c>
+      <c r="E217" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A218" s="2">
+        <v>45698</v>
+      </c>
+      <c r="B218" s="1">
+        <v>4</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D218" t="b">
+        <v>1</v>
+      </c>
+      <c r="E218" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A219" s="2">
+        <v>45698</v>
+      </c>
+      <c r="B219" s="1">
+        <v>4</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D219" t="b">
+        <v>1</v>
+      </c>
+      <c r="E219" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A220" s="2">
+        <v>45699</v>
+      </c>
+      <c r="B220" s="1">
+        <v>4</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D220" t="b">
+        <v>1</v>
+      </c>
+      <c r="E220" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A221" s="2">
+        <v>45699</v>
+      </c>
+      <c r="B221" s="1">
+        <v>4</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D221" t="b">
+        <v>1</v>
+      </c>
+      <c r="E221" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A222" s="2">
+        <v>45700</v>
+      </c>
+      <c r="B222" s="1">
+        <v>4</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D222" t="b">
+        <v>1</v>
+      </c>
+      <c r="E222" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A223" s="2">
+        <v>45700</v>
+      </c>
+      <c r="B223" s="1">
+        <v>4</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D223" t="b">
+        <v>1</v>
+      </c>
+      <c r="E223" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A224" s="2">
+        <v>45701</v>
+      </c>
+      <c r="B224" s="1">
+        <v>4</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D224" t="b">
+        <v>1</v>
+      </c>
+      <c r="E224" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A225" s="2">
+        <v>45701</v>
+      </c>
+      <c r="B225" s="1">
+        <v>4</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D225" t="b">
+        <v>1</v>
+      </c>
+      <c r="E225" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A226" s="2">
+        <v>45702</v>
+      </c>
+      <c r="B226" s="1">
+        <v>4</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D226" t="b">
+        <v>1</v>
+      </c>
+      <c r="E226" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A227" s="2">
+        <v>45702</v>
+      </c>
+      <c r="B227" s="1">
+        <v>4</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D227" t="b">
+        <v>1</v>
+      </c>
+      <c r="E227" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A228" s="2">
+        <v>45703</v>
+      </c>
+      <c r="B228" s="1">
+        <v>4</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D228" t="b">
+        <v>1</v>
+      </c>
+      <c r="E228" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A229" s="2">
+        <v>45703</v>
+      </c>
+      <c r="B229" s="1">
+        <v>4</v>
+      </c>
+      <c r="C229" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D229" t="b">
+        <v>1</v>
+      </c>
+      <c r="E229" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A230" s="2">
+        <v>45704</v>
+      </c>
+      <c r="B230" s="1">
+        <v>4</v>
+      </c>
+      <c r="C230" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D230" t="b">
+        <v>1</v>
+      </c>
+      <c r="E230" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A231" s="2">
+        <v>45704</v>
+      </c>
+      <c r="B231" s="1">
+        <v>4</v>
+      </c>
+      <c r="C231" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D231" t="b">
+        <v>1</v>
+      </c>
+      <c r="E231" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A232" s="2">
+        <v>45705</v>
+      </c>
+      <c r="B232" s="1">
+        <v>4</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D232" t="b">
+        <v>1</v>
+      </c>
+      <c r="E232" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A233" s="2">
+        <v>45705</v>
+      </c>
+      <c r="B233" s="1">
+        <v>4</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D233" t="b">
+        <v>1</v>
+      </c>
+      <c r="E233" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A234" s="2">
+        <v>45706</v>
+      </c>
+      <c r="B234" s="1">
+        <v>4</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D234" t="b">
+        <v>1</v>
+      </c>
+      <c r="E234" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A235" s="2">
+        <v>45706</v>
+      </c>
+      <c r="B235" s="1">
+        <v>4</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D235" t="b">
+        <v>1</v>
+      </c>
+      <c r="E235" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A236" s="2">
+        <v>45707</v>
+      </c>
+      <c r="B236" s="1">
+        <v>4</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D236" t="b">
+        <v>1</v>
+      </c>
+      <c r="E236" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A237" s="2">
+        <v>45707</v>
+      </c>
+      <c r="B237" s="1">
+        <v>4</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D237" t="b">
+        <v>1</v>
+      </c>
+      <c r="E237" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A238" s="2">
+        <v>45708</v>
+      </c>
+      <c r="B238" s="1">
+        <v>4</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D238" t="b">
+        <v>1</v>
+      </c>
+      <c r="E238" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A239" s="2">
+        <v>45708</v>
+      </c>
+      <c r="B239" s="1">
+        <v>4</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D239" t="b">
+        <v>1</v>
+      </c>
+      <c r="E239" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A240" s="2">
+        <v>45709</v>
+      </c>
+      <c r="B240" s="1">
+        <v>4</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D240" t="b">
+        <v>1</v>
+      </c>
+      <c r="E240" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A241" s="2">
+        <v>45709</v>
+      </c>
+      <c r="B241" s="1">
+        <v>4</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D241" t="b">
+        <v>1</v>
+      </c>
+      <c r="E241" s="4">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E73">
-    <sortCondition ref="A2:A73"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E241">
+    <sortCondition ref="A2:A241"/>
+    <sortCondition descending="1" ref="C2:C241"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>